<commit_message>
20250828 Budget file update
</commit_message>
<xml_diff>
--- a/DataSources/BudgetPivot.xlsx
+++ b/DataSources/BudgetPivot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8474a192ac48de35/Documents/Koolitused/BCS_andmetarkus_2025/Andmetarkus_git/DataSources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95C5A458-5D1F-4949-9603-DEC8DCA600EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{95C5A458-5D1F-4949-9603-DEC8DCA600EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F19EACA-9776-4D50-B4CE-9346E4A46F3B}"/>
   <bookViews>
-    <workbookView xWindow="35745" yWindow="3420" windowWidth="21600" windowHeight="12645" xr2:uid="{A448E068-D00D-4D43-BCF5-A1C382574009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A448E068-D00D-4D43-BCF5-A1C382574009}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E93814E-81F9-4C2C-94BB-2C1E76FE9B86}">
   <dimension ref="A1:BU4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="BS21" sqref="BS21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,13 +894,13 @@
         <v>20000</v>
       </c>
       <c r="BS2">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BT2">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BU2">
-        <v>20000</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.25">
@@ -1115,13 +1115,13 @@
         <v>20000</v>
       </c>
       <c r="BS3">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BT3">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BU3">
-        <v>20000</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.25">
@@ -1336,13 +1336,13 @@
         <v>20000</v>
       </c>
       <c r="BS4">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BT4">
-        <v>20000</v>
+        <v>21000</v>
       </c>
       <c r="BU4">
-        <v>20000</v>
+        <v>21000</v>
       </c>
     </row>
   </sheetData>
@@ -1351,23 +1351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="761d0801-ebf0-405d-ba89-5fd93677c3c3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D8BC7FD0AA6EEA499D9B093AC6E3EACC" ma:contentTypeVersion="9" ma:contentTypeDescription="Loo uus dokument" ma:contentTypeScope="" ma:versionID="411f39168d3a60f88cab6123ec507e65">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="761d0801-ebf0-405d-ba89-5fd93677c3c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a27d5aba181a0c08311b137ab24f3109" ns3:_="">
     <xsd:import namespace="761d0801-ebf0-405d-ba89-5fd93677c3c3"/>
@@ -1541,10 +1524,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="761d0801-ebf0-405d-ba89-5fd93677c3c3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBE3A50-6F1A-440E-B3F5-0B26957AC0AF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F257E011-7AA5-473B-9963-C74D274B0489}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="761d0801-ebf0-405d-ba89-5fd93677c3c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1566,19 +1576,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F257E011-7AA5-473B-9963-C74D274B0489}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBE3A50-6F1A-440E-B3F5-0B26957AC0AF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="761d0801-ebf0-405d-ba89-5fd93677c3c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>